<commit_message>
new excel template more clear
</commit_message>
<xml_diff>
--- a/models_template.xlsx
+++ b/models_template.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="55">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
@@ -36,13 +36,34 @@
     <t xml:space="preserve">COLUMN</t>
   </si>
   <si>
+    <t xml:space="preserve">TABLE_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FOREIGN_ENTITY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FE_PROPERTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FE_PK_TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FE_PK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FE_MODULE</t>
+  </si>
+  <si>
     <t xml:space="preserve">User</t>
   </si>
   <si>
     <t xml:space="preserve">entity</t>
   </si>
   <si>
-    <t xml:space="preserve">Entity({name: "users"})</t>
+    <t xml:space="preserve">Entity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">users</t>
   </si>
   <si>
     <t xml:space="preserve">uuid</t>
@@ -78,7 +99,10 @@
     <t xml:space="preserve">Rol</t>
   </si>
   <si>
-    <t xml:space="preserve">foreign=Rol,users,string,rol,cod</t>
+    <t xml:space="preserve">foreign</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cod</t>
   </si>
   <si>
     <t xml:space="preserve">root</t>
@@ -96,13 +120,19 @@
     <t xml:space="preserve">UserPlan[]</t>
   </si>
   <si>
-    <t xml:space="preserve">foreign_ref=UserPlan,user_id,,user_plan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entity({name: "roles"})</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cod</t>
+    <t xml:space="preserve">foreign_ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserPlan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user_plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roles</t>
   </si>
   <si>
     <t xml:space="preserve">PrimaryColumn()</t>
@@ -111,19 +141,16 @@
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">users</t>
-  </si>
-  <si>
     <t xml:space="preserve">User[]</t>
   </si>
   <si>
-    <t xml:space="preserve">foreign_ref=User,rol,,user</t>
+    <t xml:space="preserve">user</t>
   </si>
   <si>
     <t xml:space="preserve">PlanType</t>
   </si>
   <si>
-    <t xml:space="preserve">Entity({name: "plan_type"})</t>
+    <t xml:space="preserve">plan_type</t>
   </si>
   <si>
     <t xml:space="preserve">plans</t>
@@ -132,13 +159,19 @@
     <t xml:space="preserve">Plan[]</t>
   </si>
   <si>
-    <t xml:space="preserve">foreign_ref=Plan,type,,plan</t>
+    <t xml:space="preserve">Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plan</t>
   </si>
   <si>
     <t xml:space="preserve">Services</t>
   </si>
   <si>
-    <t xml:space="preserve">Entity({name: "services"})</t>
+    <t xml:space="preserve">services</t>
   </si>
   <si>
     <t xml:space="preserve">description</t>
@@ -147,28 +180,7 @@
     <t xml:space="preserve">logo</t>
   </si>
   <si>
-    <t xml:space="preserve">foreign_ref=Plan,service,,plan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UserPlan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entity({name: "user_plan"})</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">foreign=User,user_plans,string,user,uuid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">foreign=Plan,user_plans,string,plan,uuid</t>
+    <t xml:space="preserve">service</t>
   </si>
   <si>
     <t xml:space="preserve">price</t>
@@ -178,24 +190,6 @@
   </si>
   <si>
     <t xml:space="preserve">Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entity({name: "plan"})</t>
-  </si>
-  <si>
-    <t xml:space="preserve">service</t>
-  </si>
-  <si>
-    <t xml:space="preserve">foreign=Services,plans,string,services,uuid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">foreign=PlanType,plans,string,plan_type,cod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">foreign_ref=UserPlan,plan,,user_plan</t>
   </si>
 </sst>
 </file>
@@ -206,7 +200,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -244,6 +238,13 @@
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -297,7 +298,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -319,6 +320,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -410,7 +415,7 @@
   <dimension ref="A1:AMJ11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -418,7 +423,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.76"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -430,6 +438,24 @@
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="AMB1" s="1"/>
       <c r="AMC1" s="1"/>
@@ -443,112 +469,172 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>17</v>
+        <v>24</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>23</v>
+        <v>31</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -567,10 +653,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -578,10 +664,13 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.36"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -591,50 +680,115 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>30</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -655,14 +809,16 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.23"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.72"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -675,56 +831,110 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="J5" s="5"/>
     </row>
   </sheetData>
@@ -743,17 +953,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.62"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.1"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -766,77 +979,176 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -854,10 +1166,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -865,10 +1177,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.37"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="32.51"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.19"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -878,93 +1193,165 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>42</v>
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
-        <v>43</v>
+      <c r="A4" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -983,17 +1370,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.68"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1006,89 +1396,211 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
-        <v>52</v>
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>53</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
-        <v>54</v>
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>55</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>